<commit_message>
completed lesson 1-2-3-4-5 Quality Assurance lab
</commit_message>
<xml_diff>
--- a/Katalon Projects/S002.xlsx
+++ b/Katalon Projects/S002.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>No.</t>
   </si>
@@ -71,14 +71,22 @@
     <t>Authenticated User</t>
   </si>
   <si>
-    <t>Products related to the search keys will displayed properly 
-and don't show unrelated products.</t>
-  </si>
-  <si>
-    <t>As an authenticated user,  entering some keys to search related products.</t>
-  </si>
-  <si>
-    <t>As an unauthenticated user,  entering some keys to search related products.</t>
+    <t>Products related to the valid search keys will displayed properly and don't show unrelated products.</t>
+  </si>
+  <si>
+    <t>As an unauthenticated user,  entering  valid keys to search related products.</t>
+  </si>
+  <si>
+    <t>As an authenticated user,  entering valid keys to search related products.</t>
+  </si>
+  <si>
+    <t>Entering  invalid keys to search related products.</t>
+  </si>
+  <si>
+    <t>Entering invalid keys to search related products.</t>
+  </si>
+  <si>
+    <t>The system shows the message: "Không tìm thấy kết quả phù hợp!"</t>
   </si>
 </sst>
 </file>
@@ -503,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,12 +555,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>15</v>
@@ -573,29 +581,81 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>